<commit_message>
feat: included scripts to generate figures
</commit_message>
<xml_diff>
--- a/data/input_experimental.xlsx
+++ b/data/input_experimental.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon.sharepoint.com/sites/FoNS_Chemistry_RRG/Romain_Research_Group/Ryan_Reese_DigiChem_2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="11_47C5866CB8C9003B98FC07C2E17A290884E2B735" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{596CA6EB-27E7-4FDF-B8D8-99A5C90E58D6}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="11_47C5866CB8C9003B98FC07C2E17A290884E2B735" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F80F1C33-77F5-4698-B5A3-06F635413EA2}"/>
   <bookViews>
-    <workbookView xWindow="34450" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>temperature</t>
   </si>
   <si>
-    <t>monomer_conc</t>
-  </si>
-  <si>
     <t>monomer_state</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>pressure</t>
   </si>
   <si>
-    <t>solvent_conc</t>
-  </si>
-  <si>
     <t>solvent_model</t>
   </si>
   <si>
@@ -114,9 +108,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>polymer_length</t>
-  </si>
-  <si>
     <t>O=C1OCCCC1</t>
   </si>
   <si>
@@ -337,6 +328,15 @@
   </si>
   <si>
     <t>THF</t>
+  </si>
+  <si>
+    <t>repeating_units</t>
+  </si>
+  <si>
+    <t>initial_monomer_conc</t>
+  </si>
+  <si>
+    <t>bulk_monomer_conc</t>
   </si>
 </sst>
 </file>
@@ -421,6 +421,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -689,7 +693,7 @@
   <dimension ref="A1:AD68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -705,93 +709,93 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="AC1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD1" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -799,17 +803,18 @@
       <c r="F2" s="8">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>97</v>
+      <c r="G2" s="8"/>
+      <c r="H2" t="s">
+        <v>94</v>
       </c>
       <c r="I2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N2" s="8">
         <v>-12</v>
@@ -821,15 +826,15 @@
         <v>2025</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -837,17 +842,18 @@
       <c r="F3" s="8">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>97</v>
+      <c r="G3" s="8"/>
+      <c r="H3" t="s">
+        <v>94</v>
       </c>
       <c r="I3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N3" s="8">
         <v>-16.2</v>
@@ -859,15 +865,15 @@
         <v>2025</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
@@ -875,17 +881,18 @@
       <c r="F4" s="8">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>97</v>
+      <c r="G4" s="8"/>
+      <c r="H4" t="s">
+        <v>94</v>
       </c>
       <c r="I4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N4" s="8">
         <v>-4.5999999999999996</v>
@@ -897,15 +904,15 @@
         <v>2025</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -913,17 +920,18 @@
       <c r="F5" s="8">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
-        <v>97</v>
+      <c r="G5" s="8"/>
+      <c r="H5" t="s">
+        <v>94</v>
       </c>
       <c r="I5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N5" s="8">
         <v>-4.2</v>
@@ -935,15 +943,15 @@
         <v>2025</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
@@ -951,17 +959,18 @@
       <c r="F6" s="8">
         <v>2</v>
       </c>
-      <c r="G6" t="s">
-        <v>97</v>
+      <c r="G6" s="8"/>
+      <c r="H6" t="s">
+        <v>94</v>
       </c>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N6" s="8">
         <v>-0.9</v>
@@ -973,15 +982,15 @@
         <v>2025</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -989,17 +998,18 @@
       <c r="F7" s="8">
         <v>2</v>
       </c>
-      <c r="G7" t="s">
-        <v>97</v>
+      <c r="G7" s="8"/>
+      <c r="H7" t="s">
+        <v>94</v>
       </c>
       <c r="I7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N7" s="8">
         <v>-0.8</v>
@@ -1011,15 +1021,15 @@
         <v>2025</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -1027,14 +1037,15 @@
       <c r="F8" s="8">
         <v>8.61</v>
       </c>
+      <c r="G8" s="8"/>
       <c r="I8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N8" s="8">
         <v>-17.2</v>
@@ -1046,15 +1057,15 @@
         <v>2025</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
@@ -1062,14 +1073,15 @@
       <c r="F9" s="8">
         <v>7.68</v>
       </c>
+      <c r="G9" s="8"/>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N9" s="8">
         <v>-25</v>
@@ -1081,15 +1093,15 @@
         <v>2025</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
@@ -1097,14 +1109,15 @@
       <c r="F10" s="8">
         <v>8.76</v>
       </c>
+      <c r="G10" s="8"/>
       <c r="I10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N10" s="8">
         <v>-19.3</v>
@@ -1116,15 +1129,15 @@
         <v>2025</v>
       </c>
       <c r="R10" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -1132,17 +1145,18 @@
       <c r="F11" s="8">
         <v>0.2</v>
       </c>
-      <c r="G11" t="s">
-        <v>97</v>
+      <c r="G11" s="8"/>
+      <c r="H11" t="s">
+        <v>94</v>
       </c>
       <c r="I11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N11" s="8">
         <v>-16.600000000000001</v>
@@ -1154,15 +1168,15 @@
         <v>2025</v>
       </c>
       <c r="R11" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -1170,17 +1184,18 @@
       <c r="F12" s="8">
         <v>0.35</v>
       </c>
-      <c r="G12" t="s">
-        <v>98</v>
+      <c r="G12" s="8"/>
+      <c r="H12" t="s">
+        <v>95</v>
       </c>
       <c r="I12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N12" s="8">
         <v>-8.4</v>
@@ -1192,28 +1207,29 @@
         <v>2002</v>
       </c>
       <c r="R12" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
       </c>
       <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
       <c r="I13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N13" s="8">
         <v>-10.5</v>
@@ -1225,15 +1241,15 @@
         <v>1996</v>
       </c>
       <c r="R13" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -1241,17 +1257,18 @@
       <c r="F14" s="8">
         <v>2</v>
       </c>
-      <c r="G14" t="s">
-        <v>98</v>
+      <c r="G14" s="8"/>
+      <c r="H14" t="s">
+        <v>95</v>
       </c>
       <c r="I14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N14" s="8">
         <v>-14</v>
@@ -1263,28 +1280,29 @@
         <v>2002</v>
       </c>
       <c r="R14" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
       </c>
       <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
       <c r="I15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N15" s="8">
         <v>-17</v>
@@ -1296,15 +1314,15 @@
         <v>1996</v>
       </c>
       <c r="R15" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -1312,17 +1330,18 @@
       <c r="F16" s="8">
         <v>1.8</v>
       </c>
-      <c r="G16" t="s">
-        <v>98</v>
+      <c r="G16" s="8"/>
+      <c r="H16" t="s">
+        <v>95</v>
       </c>
       <c r="I16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N16" s="8">
         <v>-13.8</v>
@@ -1334,15 +1353,15 @@
         <v>2002</v>
       </c>
       <c r="R16" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -1350,17 +1369,18 @@
       <c r="F17" s="8">
         <v>0.2</v>
       </c>
-      <c r="G17" t="s">
-        <v>97</v>
+      <c r="G17" s="8"/>
+      <c r="H17" t="s">
+        <v>94</v>
       </c>
       <c r="I17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N17" s="8">
         <v>-16.8</v>
@@ -1372,28 +1392,29 @@
         <v>2005</v>
       </c>
       <c r="R17" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
       </c>
       <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
       <c r="I18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N18" s="8">
         <v>-17</v>
@@ -1405,28 +1426,29 @@
         <v>1996</v>
       </c>
       <c r="R18" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C19" t="b">
         <v>1</v>
       </c>
       <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
       <c r="I19" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J19" t="s">
+        <v>68</v>
+      </c>
+      <c r="M19" t="s">
         <v>71</v>
-      </c>
-      <c r="M19" t="s">
-        <v>74</v>
       </c>
       <c r="N19" s="8">
         <v>-5.4</v>
@@ -1438,28 +1460,29 @@
         <v>1996</v>
       </c>
       <c r="R19" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
       </c>
       <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
       <c r="I20" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J20" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N20" s="8">
         <v>-82.3</v>
@@ -1471,28 +1494,29 @@
         <v>1996</v>
       </c>
       <c r="R20" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C21" t="b">
         <v>1</v>
       </c>
       <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
       <c r="I21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J21" t="s">
+        <v>68</v>
+      </c>
+      <c r="M21" t="s">
         <v>71</v>
-      </c>
-      <c r="M21" t="s">
-        <v>74</v>
       </c>
       <c r="N21" s="8">
         <v>-75</v>
@@ -1504,28 +1528,29 @@
         <v>1996</v>
       </c>
       <c r="R21" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
       </c>
       <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
       <c r="I22" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N22" s="8">
         <v>-84</v>
@@ -1537,28 +1562,29 @@
         <v>1996</v>
       </c>
       <c r="R22" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C23" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
       <c r="I23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N23" s="8">
         <v>-7</v>
@@ -1570,28 +1596,29 @@
         <v>1996</v>
       </c>
       <c r="R23" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C24" t="b">
         <v>1</v>
       </c>
       <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
       <c r="I24" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J24" t="s">
+        <v>68</v>
+      </c>
+      <c r="M24" t="s">
         <v>71</v>
-      </c>
-      <c r="M24" t="s">
-        <v>74</v>
       </c>
       <c r="N24" s="8">
         <v>5.0999999999999996</v>
@@ -1603,28 +1630,29 @@
         <v>1996</v>
       </c>
       <c r="R24" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C25" t="b">
         <v>1</v>
       </c>
       <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
       <c r="I25" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J25" t="s">
+        <v>68</v>
+      </c>
+      <c r="M25" t="s">
         <v>71</v>
-      </c>
-      <c r="M25" t="s">
-        <v>74</v>
       </c>
       <c r="N25" s="8">
         <v>-10.5</v>
@@ -1636,28 +1664,29 @@
         <v>1996</v>
       </c>
       <c r="R25" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C26" t="b">
         <v>1</v>
       </c>
       <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
       <c r="I26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N26" s="8">
         <v>-20.9</v>
@@ -1667,28 +1696,29 @@
         <v>1980</v>
       </c>
       <c r="R26" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C27" t="b">
         <v>1</v>
       </c>
       <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
       <c r="I27" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J27" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N27" s="8">
         <v>-35</v>
@@ -1700,28 +1730,29 @@
         <v>1996</v>
       </c>
       <c r="R27" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C28" t="b">
         <v>1</v>
       </c>
       <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
       <c r="I28" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J28" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M28" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N28" s="8">
         <v>-27.4</v>
@@ -1733,28 +1764,29 @@
         <v>2009</v>
       </c>
       <c r="R28" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C29" t="b">
         <v>1</v>
       </c>
       <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
       <c r="I29" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J29" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M29" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N29" s="8">
         <v>-31</v>
@@ -1766,28 +1798,29 @@
         <v>1996</v>
       </c>
       <c r="R29" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C30" t="b">
         <v>1</v>
       </c>
       <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
       <c r="I30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J30" t="s">
+        <v>68</v>
+      </c>
+      <c r="M30" t="s">
         <v>71</v>
-      </c>
-      <c r="M30" t="s">
-        <v>74</v>
       </c>
       <c r="N30" s="8">
         <v>-17</v>
@@ -1799,28 +1832,29 @@
         <v>1996</v>
       </c>
       <c r="R30" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C31" t="b">
         <v>1</v>
       </c>
       <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
       <c r="I31" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J31" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N31" s="8">
         <v>-28.8</v>
@@ -1832,28 +1866,29 @@
         <v>2009</v>
       </c>
       <c r="R31" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C32" t="b">
         <v>1</v>
       </c>
       <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
       <c r="I32" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J32" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N32" s="8">
         <v>-37</v>
@@ -1865,28 +1900,29 @@
         <v>1996</v>
       </c>
       <c r="R32" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C33" t="b">
         <v>1</v>
       </c>
       <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
       <c r="I33" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J33" t="s">
+        <v>68</v>
+      </c>
+      <c r="M33" t="s">
         <v>71</v>
-      </c>
-      <c r="M33" t="s">
-        <v>74</v>
       </c>
       <c r="N33" s="8">
         <v>-19</v>
@@ -1898,28 +1934,29 @@
         <v>1996</v>
       </c>
       <c r="R33" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C34" t="b">
         <v>1</v>
       </c>
       <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
       <c r="I34" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J34" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M34" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N34" s="8">
         <v>-43</v>
@@ -1931,28 +1968,29 @@
         <v>1996</v>
       </c>
       <c r="R34" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C35" t="b">
         <v>1</v>
       </c>
       <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
       <c r="I35" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J35" t="s">
+        <v>68</v>
+      </c>
+      <c r="M35" t="s">
         <v>71</v>
-      </c>
-      <c r="M35" t="s">
-        <v>74</v>
       </c>
       <c r="N35" s="8">
         <v>-21</v>
@@ -1964,28 +2002,29 @@
         <v>1996</v>
       </c>
       <c r="R35" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C36" t="b">
         <v>1</v>
       </c>
       <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
       <c r="I36" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J36" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M36" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N36" s="8">
         <v>-62</v>
@@ -1997,28 +2036,29 @@
         <v>1996</v>
       </c>
       <c r="R36" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C37" t="b">
         <v>1</v>
       </c>
       <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
       <c r="I37" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J37" t="s">
+        <v>68</v>
+      </c>
+      <c r="M37" t="s">
         <v>71</v>
-      </c>
-      <c r="M37" t="s">
-        <v>74</v>
       </c>
       <c r="N37" s="8">
         <v>-28</v>
@@ -2030,28 +2070,29 @@
         <v>1996</v>
       </c>
       <c r="R37" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C38" t="b">
         <v>1</v>
       </c>
       <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
       <c r="I38" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J38" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M38" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N38" s="8">
         <v>-38</v>
@@ -2063,28 +2104,29 @@
         <v>1996</v>
       </c>
       <c r="R38" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C39" t="b">
         <v>1</v>
       </c>
       <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
       <c r="I39" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J39" t="s">
+        <v>68</v>
+      </c>
+      <c r="M39" t="s">
         <v>71</v>
-      </c>
-      <c r="M39" t="s">
-        <v>74</v>
       </c>
       <c r="N39" s="8">
         <v>2</v>
@@ -2096,28 +2138,29 @@
         <v>1996</v>
       </c>
       <c r="R39" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C40" t="b">
         <v>1</v>
       </c>
       <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
       <c r="I40" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J40" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M40" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N40" s="8">
         <v>-39</v>
@@ -2129,28 +2172,29 @@
         <v>1996</v>
       </c>
       <c r="R40" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C41" t="b">
         <v>1</v>
       </c>
       <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
       <c r="I41" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J41" t="s">
+        <v>68</v>
+      </c>
+      <c r="M41" t="s">
         <v>71</v>
-      </c>
-      <c r="M41" t="s">
-        <v>74</v>
       </c>
       <c r="N41" s="8">
         <v>10</v>
@@ -2162,28 +2206,29 @@
         <v>1996</v>
       </c>
       <c r="R41" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C42" t="b">
         <v>1</v>
       </c>
       <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
       <c r="I42" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J42" t="s">
+        <v>68</v>
+      </c>
+      <c r="M42" t="s">
         <v>71</v>
-      </c>
-      <c r="M42" t="s">
-        <v>74</v>
       </c>
       <c r="N42" s="8">
         <v>-33.409999999999997</v>
@@ -2195,28 +2240,29 @@
         <v>2018</v>
       </c>
       <c r="R42" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C43" t="b">
         <v>1</v>
       </c>
       <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
       <c r="I43" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J43" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="M43" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N43" s="8">
         <v>-19</v>
@@ -2228,15 +2274,15 @@
         <v>2015</v>
       </c>
       <c r="R43" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C44" t="b">
         <v>1</v>
@@ -2244,17 +2290,18 @@
       <c r="F44" s="8">
         <v>1</v>
       </c>
-      <c r="G44" t="s">
-        <v>99</v>
+      <c r="G44" s="8"/>
+      <c r="H44" t="s">
+        <v>96</v>
       </c>
       <c r="I44" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J44" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M44" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N44" s="8">
         <v>-22.9</v>
@@ -2266,28 +2313,29 @@
         <v>1990</v>
       </c>
       <c r="R44" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C45" t="b">
         <v>1</v>
       </c>
       <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
       <c r="I45" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J45" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M45" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N45" s="8">
         <v>-29.1</v>
@@ -2299,28 +2347,29 @@
         <v>1990</v>
       </c>
       <c r="R45" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C46" t="b">
         <v>1</v>
       </c>
       <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
       <c r="I46" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J46" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M46" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N46" s="8">
         <v>-23.3</v>
@@ -2332,28 +2381,29 @@
         <v>1997</v>
       </c>
       <c r="R46" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C47" t="b">
         <v>1</v>
       </c>
       <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
       <c r="I47" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J47" t="s">
+        <v>68</v>
+      </c>
+      <c r="M47" t="s">
         <v>71</v>
-      </c>
-      <c r="M47" t="s">
-        <v>74</v>
       </c>
       <c r="N47" s="8">
         <v>-8.6999999999999993</v>
@@ -2365,15 +2415,15 @@
         <v>1982</v>
       </c>
       <c r="R47" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C48" t="b">
         <v>1</v>
@@ -2381,14 +2431,15 @@
       <c r="F48" s="8">
         <v>6</v>
       </c>
+      <c r="G48" s="8"/>
       <c r="I48" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J48" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M48" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N48" s="8">
         <v>-12.2</v>
@@ -2400,15 +2451,15 @@
         <v>2024</v>
       </c>
       <c r="R48" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C49" t="b">
         <v>1</v>
@@ -2416,14 +2467,15 @@
       <c r="F49" s="8">
         <v>6</v>
       </c>
+      <c r="G49" s="8"/>
       <c r="I49" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J49" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M49" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N49" s="8">
         <v>-17.100000000000001</v>
@@ -2435,15 +2487,15 @@
         <v>2024</v>
       </c>
       <c r="R49" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C50" t="b">
         <v>1</v>
@@ -2451,14 +2503,15 @@
       <c r="F50" s="8">
         <v>1</v>
       </c>
+      <c r="G50" s="8"/>
       <c r="I50" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J50" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M50" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N50" s="8">
         <v>-12</v>
@@ -2470,15 +2523,15 @@
         <v>2024</v>
       </c>
       <c r="R50" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C51" t="b">
         <v>1</v>
@@ -2486,14 +2539,15 @@
       <c r="F51" s="8">
         <v>1</v>
       </c>
+      <c r="G51" s="8"/>
       <c r="I51" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J51" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M51" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N51" s="8">
         <v>-10.9</v>
@@ -2505,15 +2559,15 @@
         <v>2024</v>
       </c>
       <c r="R51" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C52" t="b">
         <v>1</v>
@@ -2521,14 +2575,15 @@
       <c r="F52" s="8">
         <v>1</v>
       </c>
+      <c r="G52" s="8"/>
       <c r="I52" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J52" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M52" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N52" s="8">
         <v>-11.4</v>
@@ -2540,15 +2595,15 @@
         <v>2024</v>
       </c>
       <c r="R52" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C53" t="b">
         <v>1</v>
@@ -2556,14 +2611,15 @@
       <c r="F53" s="8">
         <v>1</v>
       </c>
+      <c r="G53" s="8"/>
       <c r="I53" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J53" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M53" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N53" s="8">
         <v>-12.9</v>
@@ -2575,15 +2631,15 @@
         <v>2024</v>
       </c>
       <c r="R53" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C54" t="b">
         <v>1</v>
@@ -2591,14 +2647,15 @@
       <c r="F54" s="8">
         <v>1</v>
       </c>
+      <c r="G54" s="8"/>
       <c r="I54" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J54" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M54" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N54" s="8">
         <v>-12.1</v>
@@ -2610,15 +2667,15 @@
         <v>2024</v>
       </c>
       <c r="R54" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C55" t="b">
         <v>1</v>
@@ -2626,14 +2683,15 @@
       <c r="F55" s="8">
         <v>1</v>
       </c>
+      <c r="G55" s="8"/>
       <c r="I55" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J55" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M55" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N55" s="8">
         <v>-13.3</v>
@@ -2645,15 +2703,15 @@
         <v>2024</v>
       </c>
       <c r="R55" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B56" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C56" t="b">
         <v>1</v>
@@ -2661,17 +2719,18 @@
       <c r="F56" s="8">
         <v>10</v>
       </c>
-      <c r="G56" t="s">
-        <v>100</v>
+      <c r="G56" s="8"/>
+      <c r="H56" t="s">
+        <v>97</v>
       </c>
       <c r="I56" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J56" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M56" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N56" s="8">
         <v>-5.4</v>
@@ -2683,31 +2742,32 @@
         <v>2016</v>
       </c>
       <c r="R56" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C57" t="b">
         <v>1</v>
       </c>
       <c r="F57" s="8"/>
-      <c r="G57" t="s">
-        <v>101</v>
+      <c r="G57" s="8"/>
+      <c r="H57" t="s">
+        <v>98</v>
       </c>
       <c r="I57" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J57" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M57" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N57" s="8">
         <v>-15.6</v>
@@ -2719,31 +2779,32 @@
         <v>2019</v>
       </c>
       <c r="R57" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C58" t="b">
         <v>1</v>
       </c>
       <c r="F58" s="8"/>
-      <c r="G58" t="s">
-        <v>102</v>
+      <c r="G58" s="8"/>
+      <c r="H58" t="s">
+        <v>99</v>
       </c>
       <c r="I58" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J58" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M58" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N58" s="8">
         <v>-20</v>
@@ -2755,28 +2816,29 @@
         <v>2018</v>
       </c>
       <c r="R58" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B59" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C59" t="b">
         <v>1</v>
       </c>
       <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
       <c r="I59" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J59" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M59" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N59" s="8">
         <v>-13.8</v>
@@ -2788,28 +2850,29 @@
         <v>2014</v>
       </c>
       <c r="R59" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C60" t="b">
         <v>1</v>
       </c>
       <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
       <c r="I60" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J60" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M60" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N60" s="8">
         <v>-17.100000000000001</v>
@@ -2821,28 +2884,29 @@
         <v>2011</v>
       </c>
       <c r="R60" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C61" t="b">
         <v>1</v>
       </c>
       <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
       <c r="I61" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J61" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M61" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N61" s="8">
         <v>-13.8</v>
@@ -2854,28 +2918,29 @@
         <v>2003</v>
       </c>
       <c r="R61" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B62" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C62" t="b">
         <v>1</v>
       </c>
       <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
       <c r="I62" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J62" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M62" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N62" s="8">
         <v>-14.1</v>
@@ -2890,23 +2955,24 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C63" t="b">
         <v>1</v>
       </c>
       <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
       <c r="I63" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J63" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M63" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N63" s="8">
         <v>-15.8</v>
@@ -2918,28 +2984,29 @@
         <v>2001</v>
       </c>
       <c r="R63" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C64" t="b">
         <v>1</v>
       </c>
       <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
       <c r="I64" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J64" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M64" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N64" s="8">
         <v>0.4</v>
@@ -2951,28 +3018,29 @@
         <v>2009</v>
       </c>
       <c r="R64" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B65" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C65" t="b">
         <v>1</v>
       </c>
       <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
       <c r="I65" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J65" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M65" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N65" s="8">
         <v>-7.1</v>
@@ -2984,28 +3052,29 @@
         <v>2009</v>
       </c>
       <c r="R65" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B66" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C66" t="b">
         <v>1</v>
       </c>
       <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
       <c r="I66" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J66" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M66" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N66" s="8">
         <v>-13.8</v>
@@ -3017,31 +3086,32 @@
         <v>2009</v>
       </c>
       <c r="R66" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B67" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C67" t="b">
         <v>1</v>
       </c>
       <c r="F67" s="8"/>
-      <c r="G67" t="s">
-        <v>103</v>
+      <c r="G67" s="8"/>
+      <c r="H67" t="s">
+        <v>100</v>
       </c>
       <c r="I67" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J67" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M67" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N67" s="8">
         <v>-18</v>
@@ -3053,15 +3123,15 @@
         <v>2013</v>
       </c>
       <c r="R67" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B68" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C68" t="b">
         <v>1</v>
@@ -3069,17 +3139,18 @@
       <c r="F68" s="8">
         <v>5</v>
       </c>
-      <c r="G68" t="s">
-        <v>100</v>
+      <c r="G68" s="8"/>
+      <c r="H68" t="s">
+        <v>97</v>
       </c>
       <c r="I68" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J68" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M68" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N68" s="8">
         <v>-5.9</v>
@@ -3103,6 +3174,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="240bb28e-6377-48b0-832f-151ffa71870e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5f270ae-dbad-4cfd-80e2-71659db687aa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002914CBC9445B8347939C6B4510D67668" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="debcf52f3d4c81bc84586c816ca1bc65">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5f270ae-dbad-4cfd-80e2-71659db687aa" xmlns:ns3="240bb28e-6377-48b0-832f-151ffa71870e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0db2ad47acd613f43945cc47365a45bf" ns2:_="" ns3:_="">
     <xsd:import namespace="b5f270ae-dbad-4cfd-80e2-71659db687aa"/>
@@ -3331,17 +3413,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="240bb28e-6377-48b0-832f-151ffa71870e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5f270ae-dbad-4cfd-80e2-71659db687aa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E31F8A5B-9EBA-4355-A82B-5141D4A521CE}">
   <ds:schemaRefs>
@@ -3351,6 +3422,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB02FF4E-10B3-4B92-B10C-B2349DBBFE67}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="240bb28e-6377-48b0-832f-151ffa71870e"/>
+    <ds:schemaRef ds:uri="b5f270ae-dbad-4cfd-80e2-71659db687aa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C62789F9-1650-4133-931E-1E27A89DED57}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3367,21 +3455,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB02FF4E-10B3-4B92-B10C-B2349DBBFE67}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="240bb28e-6377-48b0-832f-151ffa71870e"/>
-    <ds:schemaRef ds:uri="b5f270ae-dbad-4cfd-80e2-71659db687aa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Included experimental ROR data and field for delta_g in core models
</commit_message>
<xml_diff>
--- a/data/input_experimental.xlsx
+++ b/data/input_experimental.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon.sharepoint.com/sites/FoNS_Chemistry_RRG/Romain_Research_Group/Ryan_Reese_DigiChem_2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="11_47C5866CB8C9003B98FC07C2E17A290884E2B735" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F80F1C33-77F5-4698-B5A3-06F635413EA2}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="11_47C5866CB8C9003B98FC07C2E17A290884E2B735" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{066B9F7D-300F-4B5A-81B8-7E0DFF3966ED}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35780" yWindow="1220" windowWidth="28800" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="121">
   <si>
     <t>monomer_smiles</t>
   </si>
@@ -337,16 +348,76 @@
   </si>
   <si>
     <t>bulk_monomer_conc</t>
+  </si>
+  <si>
+    <t>delta_g</t>
+  </si>
+  <si>
+    <t>ROR</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>O=C1CC(C)O1</t>
+  </si>
+  <si>
+    <t>CC1CCCOC1=O</t>
+  </si>
+  <si>
+    <t>O=C1OC(C=C)CCC1CC</t>
+  </si>
+  <si>
+    <t>O=C1OCC(C)CC1</t>
+  </si>
+  <si>
+    <t>O=C1OC(CCCC)CCC1</t>
+  </si>
+  <si>
+    <t>O=C1OC(CC)CCC1CC</t>
+  </si>
+  <si>
+    <t>O=C1OC(C=C)CC/C1=C\C</t>
+  </si>
+  <si>
+    <t>O=C1OCC2=C(C=CC=C2)C1</t>
+  </si>
+  <si>
+    <t>O=C1OC(C)CC1</t>
+  </si>
+  <si>
+    <t>O=C1OC(CCCCC)CC1</t>
+  </si>
+  <si>
+    <t>O=C1OCCC1C</t>
+  </si>
+  <si>
+    <t>CD3OD</t>
+  </si>
+  <si>
+    <t>NMR</t>
+  </si>
+  <si>
+    <t>10.1021/acs.macromol.2c01141</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -390,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -401,6 +472,7 @@
     <xf numFmtId="12" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,15 +762,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD68"/>
+  <dimension ref="A1:AE86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M70" sqref="M70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="18" max="18" width="10.15625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -748,49 +823,52 @@
         <v>11</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -822,14 +900,14 @@
       <c r="O2" s="8">
         <v>-24</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>2025</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -861,14 +939,14 @@
       <c r="O3" s="8">
         <v>-13</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>2025</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="S3" s="9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -900,14 +978,14 @@
       <c r="O4" s="8">
         <v>18</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>2025</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="S4" s="9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -939,14 +1017,14 @@
       <c r="O5" s="8">
         <v>-7.4</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>2025</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="S5" s="9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -978,14 +1056,14 @@
       <c r="O6" s="8">
         <v>2.7</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>2025</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="S6" s="9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1017,14 +1095,14 @@
       <c r="O7" s="8">
         <v>16</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>2025</v>
       </c>
-      <c r="R7" s="9" t="s">
+      <c r="S7" s="9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1044,6 +1122,9 @@
       <c r="J8" t="s">
         <v>66</v>
       </c>
+      <c r="K8">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M8" t="s">
         <v>70</v>
       </c>
@@ -1053,14 +1134,14 @@
       <c r="O8" s="8">
         <v>-40.700000000000003</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>2025</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="S8" s="9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1080,6 +1161,9 @@
       <c r="J9" t="s">
         <v>66</v>
       </c>
+      <c r="K9">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M9" t="s">
         <v>70</v>
       </c>
@@ -1089,14 +1173,14 @@
       <c r="O9" s="8">
         <v>-51.7</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>2025</v>
       </c>
-      <c r="R9" s="9" t="s">
+      <c r="S9" s="9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1116,6 +1200,9 @@
       <c r="J10" t="s">
         <v>66</v>
       </c>
+      <c r="K10">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M10" t="s">
         <v>70</v>
       </c>
@@ -1125,14 +1212,14 @@
       <c r="O10" s="8">
         <v>-62</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>2025</v>
       </c>
-      <c r="R10" s="9" t="s">
+      <c r="S10" s="9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1164,14 +1251,14 @@
       <c r="O11" s="8">
         <v>-23.9</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>2025</v>
       </c>
-      <c r="R11" s="9" t="s">
+      <c r="S11" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1203,14 +1290,14 @@
       <c r="O12" s="8">
         <v>-14.7</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>2002</v>
       </c>
-      <c r="R12" s="9" t="s">
+      <c r="S12" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1237,14 +1324,14 @@
       <c r="O13" s="8">
         <v>-15</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>1996</v>
       </c>
-      <c r="R13" s="9" t="s">
+      <c r="S13" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1276,14 +1363,14 @@
       <c r="O14" s="8">
         <v>-6</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>2002</v>
       </c>
-      <c r="R14" s="9" t="s">
+      <c r="S14" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1310,14 +1397,14 @@
       <c r="O15" s="8">
         <v>-4</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>1996</v>
       </c>
-      <c r="R15" s="9" t="s">
+      <c r="S15" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1349,14 +1436,14 @@
       <c r="O16" s="8">
         <v>-41.2</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>2002</v>
       </c>
-      <c r="R16" s="9" t="s">
+      <c r="S16" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1388,14 +1475,14 @@
       <c r="O17" s="8">
         <v>-27.4</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>2005</v>
       </c>
-      <c r="R17" s="9" t="s">
+      <c r="S17" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1413,6 +1500,9 @@
       <c r="J18" t="s">
         <v>67</v>
       </c>
+      <c r="K18">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M18" t="s">
         <v>71</v>
       </c>
@@ -1422,14 +1512,14 @@
       <c r="O18" s="8">
         <v>-3.2</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>1996</v>
       </c>
-      <c r="R18" s="9" t="s">
+      <c r="S18" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1447,6 +1537,9 @@
       <c r="J19" t="s">
         <v>68</v>
       </c>
+      <c r="K19">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M19" t="s">
         <v>71</v>
       </c>
@@ -1456,14 +1549,14 @@
       <c r="O19" s="8">
         <v>5.3</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>1996</v>
       </c>
-      <c r="R19" s="9" t="s">
+      <c r="S19" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1481,6 +1574,9 @@
       <c r="J20" t="s">
         <v>67</v>
       </c>
+      <c r="K20">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M20" t="s">
         <v>71</v>
       </c>
@@ -1490,14 +1586,14 @@
       <c r="O20" s="8">
         <v>-74</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>1996</v>
       </c>
-      <c r="R20" s="9" t="s">
+      <c r="S20" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1515,6 +1611,9 @@
       <c r="J21" t="s">
         <v>68</v>
       </c>
+      <c r="K21">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M21" t="s">
         <v>71</v>
       </c>
@@ -1524,14 +1623,14 @@
       <c r="O21" s="8">
         <v>-54</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <v>1996</v>
       </c>
-      <c r="R21" s="9" t="s">
+      <c r="S21" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1549,6 +1648,9 @@
       <c r="J22" t="s">
         <v>67</v>
       </c>
+      <c r="K22">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M22" t="s">
         <v>71</v>
       </c>
@@ -1558,14 +1660,14 @@
       <c r="O22" s="8">
         <v>-74</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <v>1996</v>
       </c>
-      <c r="R22" s="9" t="s">
+      <c r="S22" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1583,6 +1685,9 @@
       <c r="J23" t="s">
         <v>67</v>
       </c>
+      <c r="K23">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M23" t="s">
         <v>71</v>
       </c>
@@ -1592,14 +1697,14 @@
       <c r="O23" s="8">
         <v>-65</v>
       </c>
-      <c r="Q23">
+      <c r="R23">
         <v>1996</v>
       </c>
-      <c r="R23" s="9" t="s">
+      <c r="S23" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1617,6 +1722,9 @@
       <c r="J24" t="s">
         <v>68</v>
       </c>
+      <c r="K24">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M24" t="s">
         <v>71</v>
       </c>
@@ -1626,14 +1734,14 @@
       <c r="O24" s="8">
         <v>-29.9</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <v>1996</v>
       </c>
-      <c r="R24" s="9" t="s">
+      <c r="S24" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1651,6 +1759,9 @@
       <c r="J25" t="s">
         <v>68</v>
       </c>
+      <c r="K25">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M25" t="s">
         <v>71</v>
       </c>
@@ -1660,14 +1771,14 @@
       <c r="O25" s="8">
         <v>-15</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <v>1996</v>
       </c>
-      <c r="R25" s="9" t="s">
+      <c r="S25" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1685,6 +1796,9 @@
       <c r="J26" t="s">
         <v>67</v>
       </c>
+      <c r="K26">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M26" t="s">
         <v>71</v>
       </c>
@@ -1692,14 +1806,14 @@
         <v>-20.9</v>
       </c>
       <c r="O26" s="8"/>
-      <c r="Q26">
+      <c r="R26">
         <v>1980</v>
       </c>
-      <c r="R26" s="9" t="s">
+      <c r="S26" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1717,6 +1831,9 @@
       <c r="J27" t="s">
         <v>67</v>
       </c>
+      <c r="K27">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M27" t="s">
         <v>71</v>
       </c>
@@ -1726,14 +1843,14 @@
       <c r="O27" s="8">
         <v>-76</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <v>1996</v>
       </c>
-      <c r="R27" s="9" t="s">
+      <c r="S27" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1751,6 +1868,9 @@
       <c r="J28" t="s">
         <v>67</v>
       </c>
+      <c r="K28">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M28" t="s">
         <v>71</v>
       </c>
@@ -1760,14 +1880,14 @@
       <c r="O28" s="8">
         <v>-65</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <v>2009</v>
       </c>
-      <c r="R28" s="9" t="s">
+      <c r="S28" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1785,6 +1905,9 @@
       <c r="J29" t="s">
         <v>67</v>
       </c>
+      <c r="K29">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M29" t="s">
         <v>71</v>
       </c>
@@ -1794,14 +1917,14 @@
       <c r="O29" s="8">
         <v>-54</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <v>1996</v>
       </c>
-      <c r="R29" s="9" t="s">
+      <c r="S29" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1819,6 +1942,9 @@
       <c r="J30" t="s">
         <v>68</v>
       </c>
+      <c r="K30">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M30" t="s">
         <v>71</v>
       </c>
@@ -1828,14 +1954,14 @@
       <c r="O30" s="8">
         <v>-4</v>
       </c>
-      <c r="Q30">
+      <c r="R30">
         <v>1996</v>
       </c>
-      <c r="R30" s="9" t="s">
+      <c r="S30" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -1853,6 +1979,9 @@
       <c r="J31" t="s">
         <v>67</v>
       </c>
+      <c r="K31">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M31" t="s">
         <v>71</v>
       </c>
@@ -1862,14 +1991,14 @@
       <c r="O31" s="8">
         <v>-53.9</v>
       </c>
-      <c r="Q31">
+      <c r="R31">
         <v>2009</v>
       </c>
-      <c r="R31" s="9" t="s">
+      <c r="S31" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -1887,6 +2016,9 @@
       <c r="J32" t="s">
         <v>67</v>
       </c>
+      <c r="K32">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M32" t="s">
         <v>71</v>
       </c>
@@ -1896,14 +2028,14 @@
       <c r="O32" s="8">
         <v>-60</v>
       </c>
-      <c r="Q32">
+      <c r="R32">
         <v>1996</v>
       </c>
-      <c r="R32" s="9" t="s">
+      <c r="S32" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1921,6 +2053,9 @@
       <c r="J33" t="s">
         <v>68</v>
       </c>
+      <c r="K33">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M33" t="s">
         <v>71</v>
       </c>
@@ -1930,14 +2065,14 @@
       <c r="O33" s="8">
         <v>2</v>
       </c>
-      <c r="Q33">
+      <c r="R33">
         <v>1996</v>
       </c>
-      <c r="R33" s="9" t="s">
+      <c r="S33" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1955,6 +2090,9 @@
       <c r="J34" t="s">
         <v>67</v>
       </c>
+      <c r="K34">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M34" t="s">
         <v>71</v>
       </c>
@@ -1964,14 +2102,14 @@
       <c r="O34" s="8">
         <v>-61</v>
       </c>
-      <c r="Q34">
+      <c r="R34">
         <v>1996</v>
       </c>
-      <c r="R34" s="9" t="s">
+      <c r="S34" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -1989,6 +2127,9 @@
       <c r="J35" t="s">
         <v>68</v>
       </c>
+      <c r="K35">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M35" t="s">
         <v>71</v>
       </c>
@@ -1998,14 +2139,14 @@
       <c r="O35" s="8">
         <v>7</v>
       </c>
-      <c r="Q35">
+      <c r="R35">
         <v>1996</v>
       </c>
-      <c r="R35" s="9" t="s">
+      <c r="S35" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -2023,6 +2164,9 @@
       <c r="J36" t="s">
         <v>67</v>
       </c>
+      <c r="K36">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M36" t="s">
         <v>71</v>
       </c>
@@ -2032,14 +2176,14 @@
       <c r="O36" s="8">
         <v>-69</v>
       </c>
-      <c r="Q36">
+      <c r="R36">
         <v>1996</v>
       </c>
-      <c r="R36" s="9" t="s">
+      <c r="S36" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -2057,6 +2201,9 @@
       <c r="J37" t="s">
         <v>68</v>
       </c>
+      <c r="K37">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M37" t="s">
         <v>71</v>
       </c>
@@ -2066,14 +2213,14 @@
       <c r="O37" s="8">
         <v>24</v>
       </c>
-      <c r="Q37">
+      <c r="R37">
         <v>1996</v>
       </c>
-      <c r="R37" s="9" t="s">
+      <c r="S37" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -2091,6 +2238,9 @@
       <c r="J38" t="s">
         <v>67</v>
       </c>
+      <c r="K38">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M38" t="s">
         <v>71</v>
       </c>
@@ -2100,14 +2250,14 @@
       <c r="O38" s="8">
         <v>-50</v>
       </c>
-      <c r="Q38">
+      <c r="R38">
         <v>1996</v>
       </c>
-      <c r="R38" s="9" t="s">
+      <c r="S38" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -2125,6 +2275,9 @@
       <c r="J39" t="s">
         <v>68</v>
       </c>
+      <c r="K39">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M39" t="s">
         <v>71</v>
       </c>
@@ -2134,14 +2287,14 @@
       <c r="O39" s="8">
         <v>57</v>
       </c>
-      <c r="Q39">
+      <c r="R39">
         <v>1996</v>
       </c>
-      <c r="R39" s="9" t="s">
+      <c r="S39" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>29</v>
       </c>
@@ -2159,6 +2312,9 @@
       <c r="J40" t="s">
         <v>67</v>
       </c>
+      <c r="K40">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M40" t="s">
         <v>71</v>
       </c>
@@ -2168,14 +2324,14 @@
       <c r="O40" s="8">
         <v>-86</v>
       </c>
-      <c r="Q40">
+      <c r="R40">
         <v>1996</v>
       </c>
-      <c r="R40" s="9" t="s">
+      <c r="S40" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -2193,6 +2349,9 @@
       <c r="J41" t="s">
         <v>68</v>
       </c>
+      <c r="K41">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M41" t="s">
         <v>71</v>
       </c>
@@ -2202,14 +2361,14 @@
       <c r="O41" s="8">
         <v>41</v>
       </c>
-      <c r="Q41">
+      <c r="R41">
         <v>1996</v>
       </c>
-      <c r="R41" s="9" t="s">
+      <c r="S41" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -2227,6 +2386,9 @@
       <c r="J42" t="s">
         <v>68</v>
       </c>
+      <c r="K42">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M42" t="s">
         <v>71</v>
       </c>
@@ -2236,14 +2398,14 @@
       <c r="O42" s="8">
         <v>-42.69</v>
       </c>
-      <c r="Q42">
+      <c r="R42">
         <v>2018</v>
       </c>
-      <c r="R42" s="9" t="s">
+      <c r="S42" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2261,6 +2423,9 @@
       <c r="J43" t="s">
         <v>68</v>
       </c>
+      <c r="K43">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M43" t="s">
         <v>70</v>
       </c>
@@ -2270,14 +2435,14 @@
       <c r="O43" s="8">
         <v>-12</v>
       </c>
-      <c r="Q43">
+      <c r="R43">
         <v>2015</v>
       </c>
-      <c r="R43" s="9" t="s">
+      <c r="S43" s="9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -2309,14 +2474,14 @@
       <c r="O44" s="8">
         <v>-25.03</v>
       </c>
-      <c r="Q44">
+      <c r="R44">
         <v>1990</v>
       </c>
-      <c r="R44" s="9" t="s">
+      <c r="S44" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2343,14 +2508,14 @@
       <c r="O45" s="8">
         <v>-40.74</v>
       </c>
-      <c r="Q45">
+      <c r="R45">
         <v>1990</v>
       </c>
-      <c r="R45" s="9" t="s">
+      <c r="S45" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2377,14 +2542,14 @@
       <c r="O46" s="8">
         <v>-22</v>
       </c>
-      <c r="Q46">
+      <c r="R46">
         <v>1997</v>
       </c>
-      <c r="R46" s="9" t="s">
+      <c r="S46" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2402,6 +2567,9 @@
       <c r="J47" t="s">
         <v>68</v>
       </c>
+      <c r="K47">
+        <v>298.14999999999998</v>
+      </c>
       <c r="M47" t="s">
         <v>71</v>
       </c>
@@ -2411,14 +2579,14 @@
       <c r="O47" s="8">
         <v>31.3</v>
       </c>
-      <c r="Q47">
+      <c r="R47">
         <v>1982</v>
       </c>
-      <c r="R47" s="9" t="s">
+      <c r="S47" s="9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2447,14 +2615,14 @@
       <c r="O48" s="8">
         <v>-40.1</v>
       </c>
-      <c r="Q48">
+      <c r="R48">
         <v>2024</v>
       </c>
-      <c r="R48" s="9" t="s">
+      <c r="S48" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -2483,14 +2651,14 @@
       <c r="O49" s="8">
         <v>-54.4</v>
       </c>
-      <c r="Q49">
+      <c r="R49">
         <v>2024</v>
       </c>
-      <c r="R49" s="9" t="s">
+      <c r="S49" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2519,14 +2687,14 @@
       <c r="O50" s="8">
         <v>-27.2</v>
       </c>
-      <c r="Q50">
+      <c r="R50">
         <v>2024</v>
       </c>
-      <c r="R50" s="9" t="s">
+      <c r="S50" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2555,14 +2723,14 @@
       <c r="O51" s="8">
         <v>-22.5</v>
       </c>
-      <c r="Q51">
+      <c r="R51">
         <v>2024</v>
       </c>
-      <c r="R51" s="9" t="s">
+      <c r="S51" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2591,14 +2759,14 @@
       <c r="O52" s="8">
         <v>-23.3</v>
       </c>
-      <c r="Q52">
+      <c r="R52">
         <v>2024</v>
       </c>
-      <c r="R52" s="9" t="s">
+      <c r="S52" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -2627,14 +2795,14 @@
       <c r="O53" s="8">
         <v>-27.7</v>
       </c>
-      <c r="Q53">
+      <c r="R53">
         <v>2024</v>
       </c>
-      <c r="R53" s="9" t="s">
+      <c r="S53" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -2663,14 +2831,14 @@
       <c r="O54" s="8">
         <v>-25.9</v>
       </c>
-      <c r="Q54">
+      <c r="R54">
         <v>2024</v>
       </c>
-      <c r="R54" s="9" t="s">
+      <c r="S54" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -2699,14 +2867,14 @@
       <c r="O55" s="8">
         <v>-27.5</v>
       </c>
-      <c r="Q55">
+      <c r="R55">
         <v>2024</v>
       </c>
-      <c r="R55" s="9" t="s">
+      <c r="S55" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>38</v>
       </c>
@@ -2738,14 +2906,14 @@
       <c r="O56" s="8">
         <v>-39.6</v>
       </c>
-      <c r="Q56">
+      <c r="R56">
         <v>2016</v>
       </c>
-      <c r="R56" s="9" t="s">
+      <c r="S56" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -2775,14 +2943,14 @@
       <c r="O57" s="8">
         <v>-40.4</v>
       </c>
-      <c r="Q57">
+      <c r="R57">
         <v>2019</v>
       </c>
-      <c r="R57" s="9" t="s">
+      <c r="S57" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -2812,14 +2980,14 @@
       <c r="O58" s="8">
         <v>-72</v>
       </c>
-      <c r="Q58">
+      <c r="R58">
         <v>2018</v>
       </c>
-      <c r="R58" s="9" t="s">
+      <c r="S58" s="9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>47</v>
       </c>
@@ -2846,14 +3014,14 @@
       <c r="O59" s="8">
         <v>-46</v>
       </c>
-      <c r="Q59">
+      <c r="R59">
         <v>2014</v>
       </c>
-      <c r="R59" s="9" t="s">
+      <c r="S59" s="9" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>56</v>
       </c>
@@ -2880,14 +3048,14 @@
       <c r="O60" s="8">
         <v>-54</v>
       </c>
-      <c r="Q60">
+      <c r="R60">
         <v>2011</v>
       </c>
-      <c r="R60" s="9" t="s">
+      <c r="S60" s="9" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>57</v>
       </c>
@@ -2914,14 +3082,14 @@
       <c r="O61" s="8">
         <v>-45</v>
       </c>
-      <c r="Q61">
+      <c r="R61">
         <v>2003</v>
       </c>
-      <c r="R61" s="9" t="s">
+      <c r="S61" s="9" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>57</v>
       </c>
@@ -2948,12 +3116,12 @@
       <c r="O62" s="8">
         <v>-45.3</v>
       </c>
-      <c r="Q62">
+      <c r="R62">
         <v>2000</v>
       </c>
-      <c r="R62" s="9"/>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S62" s="9"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>57</v>
       </c>
@@ -2980,14 +3148,14 @@
       <c r="O63" s="8">
         <v>-50.4</v>
       </c>
-      <c r="Q63">
+      <c r="R63">
         <v>2001</v>
       </c>
-      <c r="R63" s="9" t="s">
+      <c r="S63" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>58</v>
       </c>
@@ -3014,14 +3182,14 @@
       <c r="O64" s="8">
         <v>-30.1</v>
       </c>
-      <c r="Q64">
+      <c r="R64">
         <v>2009</v>
       </c>
-      <c r="R64" s="9" t="s">
+      <c r="S64" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>59</v>
       </c>
@@ -3048,14 +3216,14 @@
       <c r="O65" s="8">
         <v>-27.6</v>
       </c>
-      <c r="Q65">
+      <c r="R65">
         <v>2009</v>
       </c>
-      <c r="R65" s="9" t="s">
+      <c r="S65" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>60</v>
       </c>
@@ -3082,14 +3250,14 @@
       <c r="O66" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="Q66">
+      <c r="R66">
         <v>2009</v>
       </c>
-      <c r="R66" s="9" t="s">
+      <c r="S66" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>61</v>
       </c>
@@ -3119,14 +3287,14 @@
       <c r="O67" s="8">
         <v>-65</v>
       </c>
-      <c r="Q67">
+      <c r="R67">
         <v>2013</v>
       </c>
-      <c r="R67" s="9" t="s">
+      <c r="S67" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>62</v>
       </c>
@@ -3159,21 +3327,697 @@
         <v>-40.1</v>
       </c>
     </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>107</v>
+      </c>
+      <c r="B69" t="s">
+        <v>105</v>
+      </c>
+      <c r="C69" t="b">
+        <v>1</v>
+      </c>
+      <c r="E69" t="s">
+        <v>106</v>
+      </c>
+      <c r="H69" t="s">
+        <v>118</v>
+      </c>
+      <c r="I69" t="s">
+        <v>65</v>
+      </c>
+      <c r="J69" t="s">
+        <v>65</v>
+      </c>
+      <c r="K69">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M69" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q69" s="8">
+        <v>-13.137760000000002</v>
+      </c>
+      <c r="R69" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S69" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="s">
+        <v>28</v>
+      </c>
+      <c r="B70" t="s">
+        <v>105</v>
+      </c>
+      <c r="C70" t="b">
+        <v>1</v>
+      </c>
+      <c r="E70" t="s">
+        <v>106</v>
+      </c>
+      <c r="H70" t="s">
+        <v>118</v>
+      </c>
+      <c r="I70" t="s">
+        <v>65</v>
+      </c>
+      <c r="J70" t="s">
+        <v>65</v>
+      </c>
+      <c r="K70">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M70" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q70" s="8">
+        <v>-10.878400000000001</v>
+      </c>
+      <c r="R70" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S70" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
+        <v>108</v>
+      </c>
+      <c r="B71" t="s">
+        <v>105</v>
+      </c>
+      <c r="C71" t="b">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>106</v>
+      </c>
+      <c r="H71" t="s">
+        <v>118</v>
+      </c>
+      <c r="I71" t="s">
+        <v>65</v>
+      </c>
+      <c r="J71" t="s">
+        <v>65</v>
+      </c>
+      <c r="K71">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M71" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q71" s="8">
+        <v>-10.878400000000001</v>
+      </c>
+      <c r="R71" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S71" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="s">
+        <v>45</v>
+      </c>
+      <c r="B72" t="s">
+        <v>105</v>
+      </c>
+      <c r="C72" t="b">
+        <v>1</v>
+      </c>
+      <c r="E72" t="s">
+        <v>106</v>
+      </c>
+      <c r="H72" t="s">
+        <v>118</v>
+      </c>
+      <c r="I72" t="s">
+        <v>65</v>
+      </c>
+      <c r="J72" t="s">
+        <v>65</v>
+      </c>
+      <c r="K72">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M72" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q72" s="8">
+        <v>-10.878400000000001</v>
+      </c>
+      <c r="R72" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S72" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="s">
+        <v>35</v>
+      </c>
+      <c r="B73" t="s">
+        <v>105</v>
+      </c>
+      <c r="C73" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" t="s">
+        <v>106</v>
+      </c>
+      <c r="H73" t="s">
+        <v>118</v>
+      </c>
+      <c r="I73" t="s">
+        <v>65</v>
+      </c>
+      <c r="J73" t="s">
+        <v>65</v>
+      </c>
+      <c r="K73">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M73" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q73" s="8">
+        <v>-10.878400000000001</v>
+      </c>
+      <c r="R73" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S73" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="s">
+        <v>27</v>
+      </c>
+      <c r="B74" t="s">
+        <v>105</v>
+      </c>
+      <c r="C74" t="b">
+        <v>1</v>
+      </c>
+      <c r="E74" t="s">
+        <v>106</v>
+      </c>
+      <c r="H74" t="s">
+        <v>118</v>
+      </c>
+      <c r="I74" t="s">
+        <v>65</v>
+      </c>
+      <c r="J74" t="s">
+        <v>65</v>
+      </c>
+      <c r="K74">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M74" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q74" s="8">
+        <v>-4.0166399999999998</v>
+      </c>
+      <c r="R74" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S74" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" t="s">
+        <v>109</v>
+      </c>
+      <c r="B75" t="s">
+        <v>105</v>
+      </c>
+      <c r="C75" t="b">
+        <v>1</v>
+      </c>
+      <c r="E75" t="s">
+        <v>106</v>
+      </c>
+      <c r="H75" t="s">
+        <v>118</v>
+      </c>
+      <c r="I75" t="s">
+        <v>65</v>
+      </c>
+      <c r="J75" t="s">
+        <v>65</v>
+      </c>
+      <c r="K75">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M75" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q75" s="8">
+        <v>-1.7154400000000001</v>
+      </c>
+      <c r="R75" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S75" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="s">
+        <v>32</v>
+      </c>
+      <c r="B76" t="s">
+        <v>105</v>
+      </c>
+      <c r="C76" t="b">
+        <v>1</v>
+      </c>
+      <c r="E76" t="s">
+        <v>106</v>
+      </c>
+      <c r="H76" t="s">
+        <v>118</v>
+      </c>
+      <c r="I76" t="s">
+        <v>65</v>
+      </c>
+      <c r="J76" t="s">
+        <v>65</v>
+      </c>
+      <c r="K76">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M76" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q76" s="8">
+        <v>-0.66944000000000004</v>
+      </c>
+      <c r="R76" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S76" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="s">
+        <v>110</v>
+      </c>
+      <c r="B77" t="s">
+        <v>105</v>
+      </c>
+      <c r="C77" t="b">
+        <v>1</v>
+      </c>
+      <c r="E77" t="s">
+        <v>106</v>
+      </c>
+      <c r="H77" t="s">
+        <v>118</v>
+      </c>
+      <c r="I77" t="s">
+        <v>65</v>
+      </c>
+      <c r="J77" t="s">
+        <v>65</v>
+      </c>
+      <c r="K77">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M77" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q77" s="8">
+        <v>4.1840000000000002E-2</v>
+      </c>
+      <c r="R77" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S77" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" t="s">
+        <v>111</v>
+      </c>
+      <c r="B78" t="s">
+        <v>105</v>
+      </c>
+      <c r="C78" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" t="s">
+        <v>106</v>
+      </c>
+      <c r="H78" t="s">
+        <v>118</v>
+      </c>
+      <c r="I78" t="s">
+        <v>65</v>
+      </c>
+      <c r="J78" t="s">
+        <v>65</v>
+      </c>
+      <c r="K78">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M78" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q78" s="8">
+        <v>4.1840000000000002E-2</v>
+      </c>
+      <c r="R78" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S78" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" t="s">
+        <v>47</v>
+      </c>
+      <c r="B79" t="s">
+        <v>105</v>
+      </c>
+      <c r="C79" t="b">
+        <v>1</v>
+      </c>
+      <c r="E79" t="s">
+        <v>106</v>
+      </c>
+      <c r="H79" t="s">
+        <v>118</v>
+      </c>
+      <c r="I79" t="s">
+        <v>65</v>
+      </c>
+      <c r="J79" t="s">
+        <v>65</v>
+      </c>
+      <c r="K79">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M79" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q79" s="8">
+        <v>1.50624</v>
+      </c>
+      <c r="R79" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S79" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" t="s">
+        <v>112</v>
+      </c>
+      <c r="B80" t="s">
+        <v>105</v>
+      </c>
+      <c r="C80" t="b">
+        <v>1</v>
+      </c>
+      <c r="E80" t="s">
+        <v>106</v>
+      </c>
+      <c r="H80" t="s">
+        <v>118</v>
+      </c>
+      <c r="I80" t="s">
+        <v>65</v>
+      </c>
+      <c r="J80" t="s">
+        <v>65</v>
+      </c>
+      <c r="K80">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M80" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q80" s="8">
+        <v>1.50624</v>
+      </c>
+      <c r="R80" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S80" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" t="s">
+        <v>113</v>
+      </c>
+      <c r="B81" t="s">
+        <v>105</v>
+      </c>
+      <c r="C81" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" t="s">
+        <v>106</v>
+      </c>
+      <c r="H81" t="s">
+        <v>118</v>
+      </c>
+      <c r="I81" t="s">
+        <v>65</v>
+      </c>
+      <c r="J81" t="s">
+        <v>65</v>
+      </c>
+      <c r="K81">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M81" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q81" s="8">
+        <v>2.2175200000000004</v>
+      </c>
+      <c r="R81" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S81" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" t="s">
+        <v>38</v>
+      </c>
+      <c r="B82" t="s">
+        <v>105</v>
+      </c>
+      <c r="C82" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" t="s">
+        <v>106</v>
+      </c>
+      <c r="H82" t="s">
+        <v>118</v>
+      </c>
+      <c r="I82" t="s">
+        <v>65</v>
+      </c>
+      <c r="J82" t="s">
+        <v>65</v>
+      </c>
+      <c r="K82">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M82" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q82" s="8">
+        <v>4.8115999999999994</v>
+      </c>
+      <c r="R82" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S82" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" t="s">
+        <v>114</v>
+      </c>
+      <c r="B83" t="s">
+        <v>105</v>
+      </c>
+      <c r="C83" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
+        <v>106</v>
+      </c>
+      <c r="H83" t="s">
+        <v>118</v>
+      </c>
+      <c r="I83" t="s">
+        <v>65</v>
+      </c>
+      <c r="J83" t="s">
+        <v>65</v>
+      </c>
+      <c r="K83">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M83" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q83" s="8">
+        <v>7.9914399999999999</v>
+      </c>
+      <c r="R83" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S83" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" t="s">
+        <v>115</v>
+      </c>
+      <c r="B84" t="s">
+        <v>105</v>
+      </c>
+      <c r="C84" t="b">
+        <v>1</v>
+      </c>
+      <c r="E84" t="s">
+        <v>106</v>
+      </c>
+      <c r="H84" t="s">
+        <v>118</v>
+      </c>
+      <c r="I84" t="s">
+        <v>65</v>
+      </c>
+      <c r="J84" t="s">
+        <v>65</v>
+      </c>
+      <c r="K84">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M84" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q84" s="8">
+        <v>9.2466400000000011</v>
+      </c>
+      <c r="R84" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S84" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" t="s">
+        <v>117</v>
+      </c>
+      <c r="B85" t="s">
+        <v>105</v>
+      </c>
+      <c r="C85" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" t="s">
+        <v>106</v>
+      </c>
+      <c r="H85" t="s">
+        <v>118</v>
+      </c>
+      <c r="I85" t="s">
+        <v>65</v>
+      </c>
+      <c r="J85" t="s">
+        <v>65</v>
+      </c>
+      <c r="K85">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M85" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q85" s="8">
+        <v>10.167120000000001</v>
+      </c>
+      <c r="R85" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S85" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" t="s">
+        <v>116</v>
+      </c>
+      <c r="B86" t="s">
+        <v>105</v>
+      </c>
+      <c r="C86" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>106</v>
+      </c>
+      <c r="H86" t="s">
+        <v>118</v>
+      </c>
+      <c r="I86" t="s">
+        <v>65</v>
+      </c>
+      <c r="J86" t="s">
+        <v>65</v>
+      </c>
+      <c r="K86">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="M86" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q86" s="8">
+        <v>10.54368</v>
+      </c>
+      <c r="R86" s="10">
+        <v>44950</v>
+      </c>
+      <c r="S86" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="240bb28e-6377-48b0-832f-151ffa71870e" xsi:nil="true"/>
@@ -3182,6 +4026,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3414,14 +4267,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E31F8A5B-9EBA-4355-A82B-5141D4A521CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB02FF4E-10B3-4B92-B10C-B2349DBBFE67}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -3434,6 +4279,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E31F8A5B-9EBA-4355-A82B-5141D4A521CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>